<commit_message>
refactoring import queue,bantuan -btn, potensi delete -btn
</commit_message>
<xml_diff>
--- a/storage/app/private/deskel/exports/akun_pengguna.xlsx
+++ b/storage/app/private/deskel/exports/akun_pengguna.xlsx
@@ -32,7 +32,7 @@
     <t>RW001</t>
   </si>
   <si>
-    <t>UAEb39</t>
+    <t>Pmgt24</t>
   </si>
   <si>
     <t>RW 002</t>
@@ -41,7 +41,7 @@
     <t>RW002</t>
   </si>
   <si>
-    <t>IK3D10</t>
+    <t>ZWMx89</t>
   </si>
   <si>
     <t>RT 001 / RW 001</t>
@@ -50,7 +50,7 @@
     <t>RT001_RW001</t>
   </si>
   <si>
-    <t>QnZx48</t>
+    <t>7DvZ84</t>
   </si>
   <si>
     <t>RT 002 / RW 001</t>
@@ -59,7 +59,7 @@
     <t>RT002_RW001</t>
   </si>
   <si>
-    <t>x2To59</t>
+    <t>Y6Pw28</t>
   </si>
   <si>
     <t>RT 003 / RW 001</t>
@@ -68,7 +68,7 @@
     <t>RT003_RW001</t>
   </si>
   <si>
-    <t>uklD74</t>
+    <t>xLEF54</t>
   </si>
   <si>
     <t>RT 004 / RW 001</t>
@@ -77,7 +77,7 @@
     <t>RT004_RW001</t>
   </si>
   <si>
-    <t>j69414</t>
+    <t>nIEq25</t>
   </si>
   <si>
     <t>RT 005 / RW 001</t>
@@ -86,7 +86,7 @@
     <t>RT005_RW001</t>
   </si>
   <si>
-    <t>6JhU40</t>
+    <t>Vbbz45</t>
   </si>
   <si>
     <t>RT 006 / RW 001</t>
@@ -95,7 +95,7 @@
     <t>RT006_RW001</t>
   </si>
   <si>
-    <t>Uaup43</t>
+    <t>qQSl25</t>
   </si>
   <si>
     <t>RT 007 / RW 001</t>
@@ -104,7 +104,7 @@
     <t>RT007_RW001</t>
   </si>
   <si>
-    <t>zVtH94</t>
+    <t>17PB68</t>
   </si>
   <si>
     <t>RT 008 / RW 001</t>
@@ -113,7 +113,7 @@
     <t>RT008_RW001</t>
   </si>
   <si>
-    <t>nvfs99</t>
+    <t>D8VV79</t>
   </si>
   <si>
     <t>RT 009 / RW 001</t>
@@ -122,7 +122,7 @@
     <t>RT009_RW001</t>
   </si>
   <si>
-    <t>Ukef10</t>
+    <t>ZLOU82</t>
   </si>
   <si>
     <t>RT 010 / RW 001</t>
@@ -131,7 +131,7 @@
     <t>RT010_RW001</t>
   </si>
   <si>
-    <t>kSrj38</t>
+    <t>DE8U13</t>
   </si>
   <si>
     <t>RT 001 / RW 002</t>
@@ -140,7 +140,7 @@
     <t>RT001_RW002</t>
   </si>
   <si>
-    <t>M9ga82</t>
+    <t>dRRw50</t>
   </si>
   <si>
     <t>RT 002 / RW 002</t>
@@ -149,7 +149,7 @@
     <t>RT002_RW002</t>
   </si>
   <si>
-    <t>jo5X37</t>
+    <t>IySy70</t>
   </si>
   <si>
     <t>RT 003 / RW 002</t>
@@ -158,7 +158,7 @@
     <t>RT003_RW002</t>
   </si>
   <si>
-    <t>P7FR18</t>
+    <t>XnNF94</t>
   </si>
   <si>
     <t>RT 004 / RW 002</t>
@@ -167,7 +167,7 @@
     <t>RT004_RW002</t>
   </si>
   <si>
-    <t>oO4242</t>
+    <t>FAgr66</t>
   </si>
   <si>
     <t>RT 005 / RW 002</t>
@@ -176,7 +176,7 @@
     <t>RT005_RW002</t>
   </si>
   <si>
-    <t>HcVk60</t>
+    <t>pyJ358</t>
   </si>
   <si>
     <t>RT 006 / RW 002</t>
@@ -185,7 +185,7 @@
     <t>RT006_RW002</t>
   </si>
   <si>
-    <t>z7cz15</t>
+    <t>tLks33</t>
   </si>
   <si>
     <t>RT 007 / RW 002</t>
@@ -194,7 +194,7 @@
     <t>RT007_RW002</t>
   </si>
   <si>
-    <t>czVt88</t>
+    <t>h7Ls63</t>
   </si>
   <si>
     <t>RT 008 / RW 002</t>
@@ -203,7 +203,7 @@
     <t>RT008_RW002</t>
   </si>
   <si>
-    <t>eozW50</t>
+    <t>0Plf66</t>
   </si>
   <si>
     <t>RT 009 / RW 002</t>
@@ -212,7 +212,7 @@
     <t>RT009_RW002</t>
   </si>
   <si>
-    <t>cQUF54</t>
+    <t>f1NL68</t>
   </si>
   <si>
     <t>RT 010 / RW 002</t>
@@ -221,7 +221,7 @@
     <t>RT010_RW002</t>
   </si>
   <si>
-    <t>2Vww15</t>
+    <t>17fc48</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
add rekapitulasi --service --filter,fix styling --btn
</commit_message>
<xml_diff>
--- a/storage/app/private/deskel/exports/akun_pengguna.xlsx
+++ b/storage/app/private/deskel/exports/akun_pengguna.xlsx
@@ -32,7 +32,7 @@
     <t>RW001</t>
   </si>
   <si>
-    <t>Pmgt24</t>
+    <t>LQr975</t>
   </si>
   <si>
     <t>RW 002</t>
@@ -41,7 +41,7 @@
     <t>RW002</t>
   </si>
   <si>
-    <t>ZWMx89</t>
+    <t>D4nA89</t>
   </si>
   <si>
     <t>RT 001 / RW 001</t>
@@ -50,7 +50,7 @@
     <t>RT001_RW001</t>
   </si>
   <si>
-    <t>7DvZ84</t>
+    <t>rFnc57</t>
   </si>
   <si>
     <t>RT 002 / RW 001</t>
@@ -59,7 +59,7 @@
     <t>RT002_RW001</t>
   </si>
   <si>
-    <t>Y6Pw28</t>
+    <t>Adjw92</t>
   </si>
   <si>
     <t>RT 003 / RW 001</t>
@@ -68,7 +68,7 @@
     <t>RT003_RW001</t>
   </si>
   <si>
-    <t>xLEF54</t>
+    <t>GbPn87</t>
   </si>
   <si>
     <t>RT 004 / RW 001</t>
@@ -77,7 +77,7 @@
     <t>RT004_RW001</t>
   </si>
   <si>
-    <t>nIEq25</t>
+    <t>B4HF61</t>
   </si>
   <si>
     <t>RT 005 / RW 001</t>
@@ -86,7 +86,7 @@
     <t>RT005_RW001</t>
   </si>
   <si>
-    <t>Vbbz45</t>
+    <t>onn418</t>
   </si>
   <si>
     <t>RT 006 / RW 001</t>
@@ -95,7 +95,7 @@
     <t>RT006_RW001</t>
   </si>
   <si>
-    <t>qQSl25</t>
+    <t>kHcD56</t>
   </si>
   <si>
     <t>RT 007 / RW 001</t>
@@ -104,7 +104,7 @@
     <t>RT007_RW001</t>
   </si>
   <si>
-    <t>17PB68</t>
+    <t>Ph0C90</t>
   </si>
   <si>
     <t>RT 008 / RW 001</t>
@@ -113,7 +113,7 @@
     <t>RT008_RW001</t>
   </si>
   <si>
-    <t>D8VV79</t>
+    <t>TUR169</t>
   </si>
   <si>
     <t>RT 009 / RW 001</t>
@@ -122,7 +122,7 @@
     <t>RT009_RW001</t>
   </si>
   <si>
-    <t>ZLOU82</t>
+    <t>Dc5A19</t>
   </si>
   <si>
     <t>RT 010 / RW 001</t>
@@ -131,7 +131,7 @@
     <t>RT010_RW001</t>
   </si>
   <si>
-    <t>DE8U13</t>
+    <t>NJi027</t>
   </si>
   <si>
     <t>RT 001 / RW 002</t>
@@ -140,7 +140,7 @@
     <t>RT001_RW002</t>
   </si>
   <si>
-    <t>dRRw50</t>
+    <t>Fvsy80</t>
   </si>
   <si>
     <t>RT 002 / RW 002</t>
@@ -149,7 +149,7 @@
     <t>RT002_RW002</t>
   </si>
   <si>
-    <t>IySy70</t>
+    <t>2arf25</t>
   </si>
   <si>
     <t>RT 003 / RW 002</t>
@@ -158,7 +158,7 @@
     <t>RT003_RW002</t>
   </si>
   <si>
-    <t>XnNF94</t>
+    <t>I9xV63</t>
   </si>
   <si>
     <t>RT 004 / RW 002</t>
@@ -167,7 +167,7 @@
     <t>RT004_RW002</t>
   </si>
   <si>
-    <t>FAgr66</t>
+    <t>wSUr83</t>
   </si>
   <si>
     <t>RT 005 / RW 002</t>
@@ -176,7 +176,7 @@
     <t>RT005_RW002</t>
   </si>
   <si>
-    <t>pyJ358</t>
+    <t>wpmm46</t>
   </si>
   <si>
     <t>RT 006 / RW 002</t>
@@ -185,7 +185,7 @@
     <t>RT006_RW002</t>
   </si>
   <si>
-    <t>tLks33</t>
+    <t>PZXC80</t>
   </si>
   <si>
     <t>RT 007 / RW 002</t>
@@ -194,7 +194,7 @@
     <t>RT007_RW002</t>
   </si>
   <si>
-    <t>h7Ls63</t>
+    <t>GVlt95</t>
   </si>
   <si>
     <t>RT 008 / RW 002</t>
@@ -203,7 +203,7 @@
     <t>RT008_RW002</t>
   </si>
   <si>
-    <t>0Plf66</t>
+    <t>KFqv86</t>
   </si>
   <si>
     <t>RT 009 / RW 002</t>
@@ -212,7 +212,7 @@
     <t>RT009_RW002</t>
   </si>
   <si>
-    <t>f1NL68</t>
+    <t>cYhB18</t>
   </si>
   <si>
     <t>RT 010 / RW 002</t>
@@ -221,7 +221,7 @@
     <t>RT010_RW002</t>
   </si>
   <si>
-    <t>17fc48</t>
+    <t>FpNf54</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
overwrite excel export --fix
</commit_message>
<xml_diff>
--- a/storage/app/private/deskel/exports/akun_pengguna.xlsx
+++ b/storage/app/private/deskel/exports/akun_pengguna.xlsx
@@ -15,16 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="69">
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>plain_password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
   <si>
     <t>RW 001</t>
   </si>
@@ -32,7 +23,7 @@
     <t>RW001</t>
   </si>
   <si>
-    <t>uo3N56</t>
+    <t>BnsV29</t>
   </si>
   <si>
     <t>RW 002</t>
@@ -41,7 +32,7 @@
     <t>RW002</t>
   </si>
   <si>
-    <t>UCdQ86</t>
+    <t>8sQK33</t>
   </si>
   <si>
     <t>RT 001 / RW 001</t>
@@ -50,7 +41,7 @@
     <t>RT001_RW001</t>
   </si>
   <si>
-    <t>R8aO87</t>
+    <t>61eW83</t>
   </si>
   <si>
     <t>RT 002 / RW 001</t>
@@ -59,7 +50,7 @@
     <t>RT002_RW001</t>
   </si>
   <si>
-    <t>HQDA25</t>
+    <t>VC0919</t>
   </si>
   <si>
     <t>RT 003 / RW 001</t>
@@ -68,7 +59,7 @@
     <t>RT003_RW001</t>
   </si>
   <si>
-    <t>CHLA75</t>
+    <t>0lgY38</t>
   </si>
   <si>
     <t>RT 004 / RW 001</t>
@@ -77,7 +68,7 @@
     <t>RT004_RW001</t>
   </si>
   <si>
-    <t>3kVD30</t>
+    <t>GOhc14</t>
   </si>
   <si>
     <t>RT 005 / RW 001</t>
@@ -86,7 +77,7 @@
     <t>RT005_RW001</t>
   </si>
   <si>
-    <t>q1UQ74</t>
+    <t>qaJc67</t>
   </si>
   <si>
     <t>RT 006 / RW 001</t>
@@ -95,7 +86,7 @@
     <t>RT006_RW001</t>
   </si>
   <si>
-    <t>LEmO21</t>
+    <t>s2Z875</t>
   </si>
   <si>
     <t>RT 007 / RW 001</t>
@@ -104,7 +95,7 @@
     <t>RT007_RW001</t>
   </si>
   <si>
-    <t>2sRy18</t>
+    <t>CnTP60</t>
   </si>
   <si>
     <t>RT 008 / RW 001</t>
@@ -113,7 +104,7 @@
     <t>RT008_RW001</t>
   </si>
   <si>
-    <t>o7ID52</t>
+    <t>NaZ421</t>
   </si>
   <si>
     <t>RT 009 / RW 001</t>
@@ -122,7 +113,7 @@
     <t>RT009_RW001</t>
   </si>
   <si>
-    <t>jp0I52</t>
+    <t>LeeY53</t>
   </si>
   <si>
     <t>RT 010 / RW 001</t>
@@ -131,7 +122,7 @@
     <t>RT010_RW001</t>
   </si>
   <si>
-    <t>EKyb51</t>
+    <t>QbE547</t>
   </si>
   <si>
     <t>RT 001 / RW 002</t>
@@ -140,7 +131,7 @@
     <t>RT001_RW002</t>
   </si>
   <si>
-    <t>o4Lw37</t>
+    <t>gLz455</t>
   </si>
   <si>
     <t>RT 002 / RW 002</t>
@@ -149,7 +140,7 @@
     <t>RT002_RW002</t>
   </si>
   <si>
-    <t>whRw27</t>
+    <t>YY4Y11</t>
   </si>
   <si>
     <t>RT 003 / RW 002</t>
@@ -158,7 +149,7 @@
     <t>RT003_RW002</t>
   </si>
   <si>
-    <t>oJFJ87</t>
+    <t>jCQY95</t>
   </si>
   <si>
     <t>RT 004 / RW 002</t>
@@ -167,7 +158,7 @@
     <t>RT004_RW002</t>
   </si>
   <si>
-    <t>AufZ72</t>
+    <t>a9jh80</t>
   </si>
   <si>
     <t>RT 005 / RW 002</t>
@@ -176,7 +167,7 @@
     <t>RT005_RW002</t>
   </si>
   <si>
-    <t>se0j41</t>
+    <t>h3AX24</t>
   </si>
   <si>
     <t>RT 006 / RW 002</t>
@@ -185,7 +176,7 @@
     <t>RT006_RW002</t>
   </si>
   <si>
-    <t>d8TJ11</t>
+    <t>GGzX42</t>
   </si>
   <si>
     <t>RT 007 / RW 002</t>
@@ -194,7 +185,7 @@
     <t>RT007_RW002</t>
   </si>
   <si>
-    <t>oxds40</t>
+    <t>nuOS65</t>
   </si>
   <si>
     <t>RT 008 / RW 002</t>
@@ -203,7 +194,7 @@
     <t>RT008_RW002</t>
   </si>
   <si>
-    <t>eZ8b13</t>
+    <t>4gNQ67</t>
   </si>
   <si>
     <t>RT 009 / RW 002</t>
@@ -212,7 +203,7 @@
     <t>RT009_RW002</t>
   </si>
   <si>
-    <t>Kplc62</t>
+    <t>BQ7h44</t>
   </si>
   <si>
     <t>RT 010 / RW 002</t>
@@ -221,7 +212,7 @@
     <t>RT010_RW002</t>
   </si>
   <si>
-    <t>GCEH40</t>
+    <t>2d0d98</t>
   </si>
 </sst>
 </file>
@@ -561,7 +552,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -809,17 +800,6 @@
       </c>
       <c r="C22" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>66</v>
-      </c>
-      <c r="B23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>